<commit_message>
write code for drawing
</commit_message>
<xml_diff>
--- a/myCode/draw_all/code/tools/land use colors.xlsx
+++ b/myCode/draw_all/code/tools/land use colors.xlsx
@@ -5,19 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EE4A80-43EB-48D7-AE40-5072ECA68FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD726AAB-D645-4645-ACC9-4C3F10F13834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
-    <sheet name="ag group" sheetId="5" r:id="rId2"/>
-    <sheet name="non-ag" sheetId="2" r:id="rId3"/>
-    <sheet name="am" sheetId="3" r:id="rId4"/>
-    <sheet name="lu" sheetId="4" r:id="rId5"/>
+    <sheet name="ag_group" sheetId="5" r:id="rId2"/>
+    <sheet name="ag_group_map" sheetId="6" r:id="rId3"/>
+    <sheet name="non_ag" sheetId="2" r:id="rId4"/>
+    <sheet name="am" sheetId="3" r:id="rId5"/>
+    <sheet name="lu" sheetId="4" r:id="rId6"/>
+    <sheet name="food" sheetId="7" r:id="rId7"/>
+    <sheet name="water" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="147">
   <si>
     <t>code</t>
   </si>
@@ -117,12 +120,6 @@
     <t>Tropical stone fruit</t>
   </si>
   <si>
-    <t>Unallocated - modified</t>
-  </si>
-  <si>
-    <t>Unallocated - natural</t>
-  </si>
-  <si>
     <t>Vegetables</t>
   </si>
   <si>
@@ -165,27 +162,6 @@
     <t>#C8C8C8</t>
   </si>
   <si>
-    <t>Environmental Plantings</t>
-  </si>
-  <si>
-    <t>Riparian Plantings</t>
-  </si>
-  <si>
-    <t>Sheep Agroforestry</t>
-  </si>
-  <si>
-    <t>Beef Agroforestry</t>
-  </si>
-  <si>
-    <t>Carbon Plantings (Block)</t>
-  </si>
-  <si>
-    <t>Sheep Carbon Plantings</t>
-  </si>
-  <si>
-    <t>Beef Carbon Plantings</t>
-  </si>
-  <si>
     <t>BECCS</t>
   </si>
   <si>
@@ -258,71 +234,272 @@
     <t>Other land-use</t>
   </si>
   <si>
-    <t>#8B0000</t>
-  </si>
-  <si>
-    <t>#D2B48C</t>
-  </si>
-  <si>
-    <t>#8B4513</t>
-  </si>
-  <si>
-    <t>#FFA500</t>
-  </si>
-  <si>
-    <t>#A52A2A</t>
-  </si>
-  <si>
-    <t>#808000</t>
+    <t>#7298C7</t>
+  </si>
+  <si>
+    <t>#FFFF00</t>
+  </si>
+  <si>
+    <t>Transition</t>
+  </si>
+  <si>
+    <t>#D2E0FB</t>
+  </si>
+  <si>
+    <t>Environmental plantings</t>
+  </si>
+  <si>
+    <t>Riparian plantings</t>
+  </si>
+  <si>
+    <t>Sheep agroforestry</t>
+  </si>
+  <si>
+    <t>Beef agroforestry</t>
+  </si>
+  <si>
+    <t>Carbon plantings (Block)</t>
+  </si>
+  <si>
+    <t>Sheep carbon plantings (Belt)</t>
+  </si>
+  <si>
+    <t>Beef carbon plantings (Belt)</t>
+  </si>
+  <si>
+    <t>#1f77b4</t>
+  </si>
+  <si>
+    <t>#aec7e8</t>
+  </si>
+  <si>
+    <t>#ff7f0e</t>
+  </si>
+  <si>
+    <t>#ffbb78</t>
+  </si>
+  <si>
+    <t>#2ca02c</t>
+  </si>
+  <si>
+    <t>#98df8a</t>
+  </si>
+  <si>
+    <t>#d62728</t>
+  </si>
+  <si>
+    <t>#ff9896</t>
+  </si>
+  <si>
+    <t>#9467bd</t>
+  </si>
+  <si>
+    <t>#c5b0d5</t>
+  </si>
+  <si>
+    <t>#8c564b</t>
+  </si>
+  <si>
+    <t>#c49c94</t>
+  </si>
+  <si>
+    <t>#e377c2</t>
+  </si>
+  <si>
+    <t>#f7b6d2</t>
+  </si>
+  <si>
+    <t>#7f7f7f</t>
+  </si>
+  <si>
+    <t>#c7c7c7</t>
+  </si>
+  <si>
+    <t>#bcbd22</t>
+  </si>
+  <si>
+    <t>#dbdb8d</t>
+  </si>
+  <si>
+    <t>#17becf</t>
+  </si>
+  <si>
+    <t>#9edae5</t>
+  </si>
+  <si>
+    <t>#393b79</t>
+  </si>
+  <si>
+    <t>#5254a3</t>
+  </si>
+  <si>
+    <t>#6b6ecf</t>
+  </si>
+  <si>
+    <t>#637939</t>
+  </si>
+  <si>
+    <t>#8ca252</t>
+  </si>
+  <si>
+    <t>#de9ed6</t>
+  </si>
+  <si>
+    <t>Beef Lexp</t>
+  </si>
+  <si>
+    <t>Beef Meat</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Other Non-Cereal Crops</t>
+  </si>
+  <si>
+    <t>Plantation Fruit</t>
+  </si>
+  <si>
+    <t>Sheep Lexp</t>
+  </si>
+  <si>
+    <t>Sheep Meat</t>
+  </si>
+  <si>
+    <t>Sheep Wool</t>
+  </si>
+  <si>
+    <t>Stone Fruit</t>
+  </si>
+  <si>
+    <t>Summer Cereals</t>
+  </si>
+  <si>
+    <t>Summer Legumes</t>
+  </si>
+  <si>
+    <t>Summer Oilseeds</t>
+  </si>
+  <si>
+    <t>Tropical Stone Fruit</t>
+  </si>
+  <si>
+    <t>Winter Cereals</t>
+  </si>
+  <si>
+    <t>Winter Legumes</t>
+  </si>
+  <si>
+    <t>Winter Oilseeds</t>
+  </si>
+  <si>
+    <t>#b5cf6b</t>
+  </si>
+  <si>
+    <t>#cedb9c</t>
+  </si>
+  <si>
+    <t>#8c6d31</t>
+  </si>
+  <si>
+    <t>Tanami-Timor Sea Coast</t>
+  </si>
+  <si>
+    <t>#3182bd</t>
+  </si>
+  <si>
+    <t>South Western Plateau</t>
+  </si>
+  <si>
+    <t>#6baed6</t>
+  </si>
+  <si>
+    <t>South West Coast</t>
+  </si>
+  <si>
+    <t>#9ecae1</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>#c6dbef</t>
+  </si>
+  <si>
+    <t>South East Coast (Victoria)</t>
+  </si>
+  <si>
+    <t>#e6550d</t>
+  </si>
+  <si>
+    <t>South Australian Gulf</t>
+  </si>
+  <si>
+    <t>#fd8d3c</t>
+  </si>
+  <si>
+    <t>Murray-Darling Basin</t>
+  </si>
+  <si>
+    <t>#fdae6b</t>
+  </si>
+  <si>
+    <t>Pilbara-Gascoyne</t>
+  </si>
+  <si>
+    <t>#fdd0a2</t>
+  </si>
+  <si>
+    <t>North Western Plateau</t>
+  </si>
+  <si>
+    <t>#31a354</t>
+  </si>
+  <si>
+    <t>South East Coast (NSW)</t>
+  </si>
+  <si>
+    <t>#74c476</t>
+  </si>
+  <si>
+    <t>Carpentaria Coast</t>
+  </si>
+  <si>
+    <t>#a1d99b</t>
+  </si>
+  <si>
+    <t>Lake Eyre Basin</t>
+  </si>
+  <si>
+    <t>#c7e9c0</t>
+  </si>
+  <si>
+    <t>North East Coast</t>
+  </si>
+  <si>
+    <t>#756bb1</t>
   </si>
   <si>
     <t>#A9A9A9</t>
   </si>
   <si>
-    <t>#87CEEB</t>
-  </si>
-  <si>
-    <t>#CD5C5C</t>
-  </si>
-  <si>
-    <t>#BC8F8F</t>
-  </si>
-  <si>
-    <t>#CD853F</t>
-  </si>
-  <si>
-    <t>#DEB887</t>
-  </si>
-  <si>
-    <t>#A0522D</t>
-  </si>
-  <si>
-    <t>#D2691E</t>
-  </si>
-  <si>
-    <t>#4682B4</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
-    <t>#FFD700</t>
-  </si>
-  <si>
-    <t>#7298C7</t>
-  </si>
-  <si>
-    <t>#FFFF00</t>
+    <t>No agricultural management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -687,10 +864,13 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -708,10 +888,10 @@
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +899,10 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +924,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,7 +968,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +979,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +1001,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,7 +1012,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -843,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -854,7 +1034,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -865,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +1056,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -887,7 +1067,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,7 +1078,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,7 +1089,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,7 +1100,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,7 +1111,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,7 +1122,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,7 +1133,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,7 +1144,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,10 +1152,10 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,10 +1163,10 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,10 +1174,10 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,10 +1185,10 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,10 +1196,10 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,13 +1207,14 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1042,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542D8A7D-3A34-4AE5-8DF9-937CC1CA2F8F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1061,42 +1242,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1105,11 +1286,367 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03998123-DD7C-419B-B0BE-8EDD79757136}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,10 +1670,10 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,10 +1681,10 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,10 +1692,10 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,10 +1703,10 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,10 +1714,10 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,10 +1725,10 @@
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1199,10 +1736,10 @@
         <v>106</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1210,10 +1747,32 @@
         <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1222,12 +1781,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,10 +1807,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,10 +1818,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,10 +1829,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,10 +1840,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,10 +1851,32 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1303,12 +1884,304 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043FD979-195F-4385-BB3B-446A90186897}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1150A691-DE1D-456C-B1D8-8D8F96E1B7AE}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FE7CEB-5A38-4639-9585-CECD474B9183}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,26 +2196,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draw stacked area graphs
</commit_message>
<xml_diff>
--- a/myCode/draw_all/code/tools/land use colors.xlsx
+++ b/myCode/draw_all/code/tools/land use colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4E4F3-3331-4152-97DA-69F14AC7796A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA9284-8F88-4348-BFF6-87C99B1FE758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2880" windowWidth="38700" windowHeight="14565" activeTab="6" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="23040" windowHeight="14565" activeTab="5" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -24,28 +24,17 @@
     <sheet name="food" sheetId="7" r:id="rId9"/>
     <sheet name="water" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="177">
   <si>
     <t>code</t>
   </si>
@@ -482,9 +471,6 @@
     <t>#F45B5B</t>
   </si>
   <si>
-    <t>#FF7F0E</t>
-  </si>
-  <si>
     <t>Public land</t>
   </si>
   <si>
@@ -527,9 +513,6 @@
     <t>Agricultural technology (energy)</t>
   </si>
   <si>
-    <t>Environmental plantings (mixed species)</t>
-  </si>
-  <si>
     <t>Riparian buffer restoration (mixed species)</t>
   </si>
   <si>
@@ -573,13 +556,24 @@
   </si>
   <si>
     <t>#D4A59A</t>
+  </si>
+  <si>
+    <t>#AD732B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Environmental plantings (mixed local native species)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#CDFEFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +585,13 @@
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1432,6 +1433,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1441,7 +1443,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1480,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1498,6 +1500,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1854,6 +1857,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1863,7 +1867,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1886,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,7 +1900,7 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,7 +1914,7 @@
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,7 +1928,7 @@
         <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,7 +1942,7 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,7 +1956,7 @@
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +1970,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,7 +1984,7 @@
         <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,7 +1998,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,6 +2030,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2052,7 +2057,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,10 +2068,10 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2080,7 +2085,7 @@
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,10 +2096,10 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,7 +2113,7 @@
         <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2122,7 +2127,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,6 +2173,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2176,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043FD979-195F-4385-BB3B-446A90186897}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,7 +2204,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2206,7 +2212,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,21 +2233,22 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2250,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61CAFA-DABC-40F0-B6E6-C2D5A426B2B8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2266,21 +2273,22 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2305,10 +2313,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2316,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2324,7 +2332,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2332,10 +2340,11 @@
         <v>0.5</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2570,6 +2579,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: bug in data.py
</commit_message>
<xml_diff>
--- a/myCode/draw_all/code/tools/land use colors.xlsx
+++ b/myCode/draw_all/code/tools/land use colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FA7C63-1DDF-4142-9272-5ECF80FF8CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3A4252-3CDF-400C-8669-66331CFBA712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="105" windowWidth="21540" windowHeight="10065" activeTab="1" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="3585" yWindow="3750" windowWidth="12300" windowHeight="14400" firstSheet="2" activeTab="3" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="186">
   <si>
     <t>code</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Savanna burning</t>
   </si>
   <si>
-    <t>#d69dbc</t>
-  </si>
-  <si>
     <t>AgTech EI</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Other land-use</t>
   </si>
   <si>
-    <t>#7298C7</t>
-  </si>
-  <si>
     <t>#FFFF00</t>
   </si>
   <si>
@@ -535,9 +529,6 @@
   </si>
   <si>
     <t>#00a9ee</t>
-  </si>
-  <si>
-    <t>#00cf6f</t>
   </si>
   <si>
     <t>#FFCCDD</t>
@@ -566,6 +557,42 @@
   </si>
   <si>
     <t>#AD732B</t>
+  </si>
+  <si>
+    <t>Destocked - natural land</t>
+  </si>
+  <si>
+    <t>#A0522D</t>
+  </si>
+  <si>
+    <t>HIR - Beef</t>
+  </si>
+  <si>
+    <t>HIR - Sheep</t>
+  </si>
+  <si>
+    <t>#20B2AA</t>
+  </si>
+  <si>
+    <t>#CBE86B</t>
+  </si>
+  <si>
+    <t>#FEC7C7</t>
+  </si>
+  <si>
+    <t>#A14189</t>
+  </si>
+  <si>
+    <t>#4EB59F</t>
+  </si>
+  <si>
+    <t>Human-Induced Regeneration (beef)</t>
+  </si>
+  <si>
+    <t>Human-Induced Regeneration (sheep)</t>
+  </si>
+  <si>
+    <t>Destocked (natural land)</t>
   </si>
 </sst>
 </file>
@@ -978,7 +1005,7 @@
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -989,7 +1016,7 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -1003,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1025,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,7 +1074,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1058,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1069,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,7 +1107,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,7 +1118,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,7 +1129,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,7 +1151,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,7 +1162,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,7 +1173,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,7 +1184,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,7 +1195,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1179,7 +1206,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,7 +1217,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1201,7 +1228,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1212,7 +1239,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1250,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,7 +1261,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,7 +1272,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,7 +1283,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1267,7 +1294,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,7 +1305,7 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1289,7 +1316,7 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,7 +1327,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1329,106 +1356,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542D8A7D-3A34-4AE5-8DF9-937CC1CA2F8F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1479,7 +1506,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1522,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1541,10 +1568,10 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1863,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,7 +1912,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,13 +1920,13 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,13 +1934,13 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,13 +1948,13 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,13 +1962,13 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,13 +1976,13 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,13 +1990,13 @@
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,13 +2004,13 @@
         <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,38 +2021,52 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>-1</v>
       </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2037,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,10 +2108,10 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,7 +2125,7 @@
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,10 +2136,10 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,10 +2150,10 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,13 +2161,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,41 +2175,69 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>-1</v>
       </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2272,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,7 +2280,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,26 +2293,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2272,18 +2341,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2312,10 +2381,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2323,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2331,7 +2400,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2339,7 +2408,7 @@
         <v>0.5</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2374,23 +2443,23 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2467,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,15 +2475,15 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2422,7 +2491,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2430,7 +2499,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,15 +2507,15 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,15 +2523,15 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,39 +2539,39 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,39 +2579,39 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,31 +2619,31 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: run in hpc
</commit_message>
<xml_diff>
--- a/myCode/draw_all/code/tools/land use colors.xlsx
+++ b/myCode/draw_all/code/tools/land use colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3A4252-3CDF-400C-8669-66331CFBA712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D127DAA6-C642-486A-A40E-19AA48B4F35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="3750" windowWidth="12300" windowHeight="14400" firstSheet="2" activeTab="3" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25920" windowHeight="20085" firstSheet="2" activeTab="4" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,11 +2080,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2136,7 +2139,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
         <v>154</v>
@@ -2150,7 +2153,7 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
update: run task for paper2 res3
</commit_message>
<xml_diff>
--- a/myCode/draw_all/code/tools/land use colors.xlsx
+++ b/myCode/draw_all/code/tools/land use colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1AACC7-AEED-472A-8194-FF1ED916EADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A46CE48-30AA-4CF0-8E48-FBB23A6B2F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="20085" activeTab="2" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="185">
   <si>
     <t>code</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>#FFC87C</t>
-  </si>
-  <si>
-    <t>#DBE4AD</t>
   </si>
   <si>
     <t>#FEFED2</t>
@@ -1005,10 +1002,10 @@
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,10 +1013,10 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1030,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1052,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,7 +1060,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1074,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1085,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,7 +1093,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1140,7 +1137,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1151,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1159,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1173,7 +1170,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1192,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1203,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,7 +1214,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,7 +1236,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1247,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,7 +1258,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,7 +1269,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1283,7 +1280,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1294,7 +1291,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1302,7 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,7 +1313,7 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,7 +1324,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1356,106 +1353,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
         <v>113</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
         <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
         <v>121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
         <v>123</v>
-      </c>
-      <c r="B7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
         <v>125</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
         <v>127</v>
-      </c>
-      <c r="B9" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
         <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
         <v>131</v>
-      </c>
-      <c r="B11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
         <v>133</v>
-      </c>
-      <c r="B12" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
         <v>135</v>
-      </c>
-      <c r="B13" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
         <v>137</v>
-      </c>
-      <c r="B14" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1503,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1514,7 +1511,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1522,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1535,11 +1532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03998123-DD7C-419B-B0BE-8EDD79757136}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1557,10 +1557,10 @@
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,10 +1568,10 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,13 +1920,13 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +1976,13 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,13 @@
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,13 +2004,13 @@
         <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,13 +2018,13 @@
         <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,13 +2032,13 @@
         <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,13 +2046,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,13 +2060,13 @@
         <v>-1</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2080,7 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2100,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,13 +2108,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2122,13 +2122,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2136,13 +2136,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2150,13 +2150,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,13 +2164,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2178,13 +2178,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
-        <v>142</v>
-      </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2192,13 +2192,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2206,13 +2206,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2220,13 +2220,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2234,13 +2234,13 @@
         <v>-1</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2272,50 +2272,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2344,18 +2344,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
         <v>168</v>
-      </c>
-      <c r="B3" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>0.5</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2446,23 +2446,23 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,7 +2470,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,15 +2478,15 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,15 +2510,15 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,15 +2526,15 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2542,39 +2542,39 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2582,39 +2582,39 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,31 +2622,31 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>